<commit_message>
reporte de impuestos y otras correcciones
</commit_message>
<xml_diff>
--- a/dfpyme/Movimiento producto.xlsx
+++ b/dfpyme/Movimiento producto.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
   <si>
     <t>Fecha</t>
   </si>
@@ -45,45 +45,6 @@
   </si>
   <si>
     <t xml:space="preserve">Notal </t>
-  </si>
-  <si>
-    <t>2024-11-06</t>
-  </si>
-  <si>
-    <t>11:28 AM</t>
-  </si>
-  <si>
-    <t>Compra proveedor</t>
-  </si>
-  <si>
-    <t>152/COCA COLA ZERO</t>
-  </si>
-  <si>
-    <t>USUARIO ADMINISTRADOR</t>
-  </si>
-  <si>
-    <t>11:38 AM</t>
-  </si>
-  <si>
-    <t>11:41 AM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Factuta venta electrónica </t>
-  </si>
-  <si>
-    <t>Producto venta</t>
-  </si>
-  <si>
-    <t>11:55 AM</t>
-  </si>
-  <si>
-    <t>COMPRA PROVEEDOR</t>
-  </si>
-  <si>
-    <t>Entrada proveedor</t>
-  </si>
-  <si>
-    <t>12:33 PM</t>
   </si>
 </sst>
 </file>
@@ -456,7 +417,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1:J1"/>
@@ -496,189 +457,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>11</v>
-      </c>
-      <c r="G3">
-        <v>12</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4">
-        <v>12</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>13</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5">
-        <v>13</v>
-      </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
-      <c r="G5">
-        <v>10</v>
-      </c>
-      <c r="H5">
-        <v>4069</v>
-      </c>
-      <c r="I5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6">
-        <v>10</v>
-      </c>
-      <c r="F6">
-        <v>20</v>
-      </c>
-      <c r="G6">
-        <v>30</v>
-      </c>
-      <c r="H6">
-        <v>32</v>
-      </c>
-      <c r="I6" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7">
-        <v>30</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>29</v>
-      </c>
-      <c r="H7">
-        <v>4070</v>
-      </c>
-      <c r="I7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" t="s">
-        <v>18</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>